<commit_message>
ran numbers of geolocated tweets
</commit_message>
<xml_diff>
--- a/tweets_count.xlsx
+++ b/tweets_count.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uninorte-my.sharepoint.com/personal/josephmartinez_uninorte_edu_co/Documents/Scripts VMASC/Academic Research Twitter Search (10M)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olddominion-my.sharepoint.com/personal/jmart130_odu_edu/Documents/GitHub/twitter_analysis_col/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{FAA8B4CC-F93A-4FB4-865F-B9ADC0F5DF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC421BC-EC99-4320-9D3D-F3160C95A682}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AEE9D0BD-06B8-465C-A72B-F93AD1544B8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AEE9D0BD-06B8-465C-A72B-F93AD1544B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,12 +135,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5006,22 +5000,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFAC237-816D-4AA2-98E4-78987FE75B01}">
   <dimension ref="B1:S103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F77" sqref="F2:F77"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.21875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5047,7 +5041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2014</v>
       </c>
@@ -5069,7 +5063,7 @@
         <v>0.50370833333333342</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2014</v>
       </c>
@@ -5091,7 +5085,7 @@
         <v>2.0317500000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2014</v>
       </c>
@@ -5113,7 +5107,7 @@
         <v>0.68629166666666674</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2014</v>
       </c>
@@ -5135,7 +5129,7 @@
         <v>0.84962500000000007</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2014</v>
       </c>
@@ -5164,7 +5158,7 @@
         <v>0.39229166666666665</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2014</v>
       </c>
@@ -5193,7 +5187,7 @@
         <v>0.7466666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2014</v>
       </c>
@@ -5222,7 +5216,7 @@
         <v>1.0444583333333335</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2014</v>
       </c>
@@ -5251,7 +5245,7 @@
         <v>0.82629166666666665</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2014</v>
       </c>
@@ -5277,7 +5271,7 @@
         <v>1.4807916666666667</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2014</v>
       </c>
@@ -5303,7 +5297,7 @@
         <v>0.61833333333333329</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2014</v>
       </c>
@@ -5329,7 +5323,7 @@
         <v>0.71866666666666679</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2014</v>
       </c>
@@ -5355,7 +5349,7 @@
         <v>0.59879166666666672</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2015</v>
       </c>
@@ -5381,7 +5375,7 @@
         <v>0.672875</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2015</v>
       </c>
@@ -5407,7 +5401,7 @@
         <v>0.61716666666666675</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2015</v>
       </c>
@@ -5433,7 +5427,7 @@
         <v>0.77349999999999997</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2015</v>
       </c>
@@ -5459,7 +5453,7 @@
         <v>0.77729166666666671</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2015</v>
       </c>
@@ -5485,7 +5479,7 @@
         <v>1.2448333333333335</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2015</v>
       </c>
@@ -5511,7 +5505,7 @@
         <v>2.0524583333333335</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>2015</v>
       </c>
@@ -5537,7 +5531,7 @@
         <v>0.67666666666666664</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>2015</v>
       </c>
@@ -5563,7 +5557,7 @@
         <v>3.3133333333333335</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>2015</v>
       </c>
@@ -5589,7 +5583,7 @@
         <v>2.5334166666666671</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>2015</v>
       </c>
@@ -5619,7 +5613,7 @@
         <v>0.65797409474761237</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>2015</v>
       </c>
@@ -5645,7 +5639,7 @@
         <v>1.3830833333333334</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>2015</v>
       </c>
@@ -5671,7 +5665,7 @@
         <v>0.95404166666666668</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>2016</v>
       </c>
@@ -5697,7 +5691,7 @@
         <v>0.50137500000000002</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>2016</v>
       </c>
@@ -5723,7 +5717,7 @@
         <v>0.71137500000000009</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2016</v>
       </c>
@@ -5749,7 +5743,7 @@
         <v>1.2296666666666667</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>2016</v>
       </c>
@@ -5775,7 +5769,7 @@
         <v>0.49525000000000002</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>2016</v>
       </c>
@@ -5801,7 +5795,7 @@
         <v>2.3435416666666669</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>2016</v>
       </c>
@@ -5827,7 +5821,7 @@
         <v>1.4204166666666667</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>2016</v>
       </c>
@@ -5866,7 +5860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2016</v>
       </c>
@@ -5906,7 +5900,7 @@
         <v>35992</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2016</v>
       </c>
@@ -5939,7 +5933,7 @@
         <v>56593</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2016</v>
       </c>
@@ -5972,7 +5966,7 @@
         <v>76220</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2016</v>
       </c>
@@ -6008,7 +6002,7 @@
         <v>223665</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>2016</v>
       </c>
@@ -6052,7 +6046,7 @@
         <v>1461166</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2017</v>
       </c>
@@ -6096,7 +6090,7 @@
         <v>1848111</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2017</v>
       </c>
@@ -6137,7 +6131,7 @@
         <v>1480411</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2017</v>
       </c>
@@ -6170,7 +6164,7 @@
         <v>1196008</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2017</v>
       </c>
@@ -6196,7 +6190,7 @@
         <v>2.6372500000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2017</v>
       </c>
@@ -6222,7 +6216,7 @@
         <v>3.8858750000000004</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2017</v>
       </c>
@@ -6248,7 +6242,7 @@
         <v>1.3673333333333335</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>2017</v>
       </c>
@@ -6274,7 +6268,7 @@
         <v>8.4568750000000001</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>2017</v>
       </c>
@@ -6300,7 +6294,7 @@
         <v>9.7393333333333327</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>2017</v>
       </c>
@@ -6326,7 +6320,7 @@
         <v>4.8533333333333335</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>2017</v>
       </c>
@@ -6352,7 +6346,7 @@
         <v>3.4860000000000002</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>2017</v>
       </c>
@@ -6378,7 +6372,7 @@
         <v>5.4034166666666668</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>2017</v>
       </c>
@@ -6404,7 +6398,7 @@
         <v>4.9665000000000008</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>2018</v>
       </c>
@@ -6430,7 +6424,7 @@
         <v>14.730625</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>2018</v>
       </c>
@@ -6456,7 +6450,7 @@
         <v>28.678416666666667</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>2018</v>
       </c>
@@ -6482,7 +6476,7 @@
         <v>30.040208333333332</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>2018</v>
       </c>
@@ -6508,7 +6502,7 @@
         <v>17.912125</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>2018</v>
       </c>
@@ -6534,7 +6528,7 @@
         <v>15.179500000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>2018</v>
       </c>
@@ -6560,7 +6554,7 @@
         <v>17.680250000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>2018</v>
       </c>
@@ -6586,7 +6580,7 @@
         <v>12.287333333333335</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>2018</v>
       </c>
@@ -6612,7 +6606,7 @@
         <v>72.174958333333336</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>2018</v>
       </c>
@@ -6638,7 +6632,7 @@
         <v>73.01495833333334</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>2018</v>
       </c>
@@ -6664,7 +6658,7 @@
         <v>67.613583333333338</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>2018</v>
       </c>
@@ -6690,7 +6684,7 @@
         <v>46.362749999999998</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>2018</v>
       </c>
@@ -6716,7 +6710,7 @@
         <v>30.498708333333337</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>2019</v>
       </c>
@@ -6742,7 +6736,7 @@
         <v>46.420208333333335</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>2019</v>
       </c>
@@ -6768,7 +6762,7 @@
         <v>65.893916666666669</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>2019</v>
       </c>
@@ -6794,7 +6788,7 @@
         <v>54.021041666666669</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>2019</v>
       </c>
@@ -6820,7 +6814,7 @@
         <v>40.116125000000004</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>2019</v>
       </c>
@@ -6846,7 +6840,7 @@
         <v>33.412750000000003</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>2019</v>
       </c>
@@ -6872,7 +6866,7 @@
         <v>64.647625000000005</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>2019</v>
       </c>
@@ -6898,7 +6892,7 @@
         <v>38.514291666666672</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>2019</v>
       </c>
@@ -6924,7 +6918,7 @@
         <v>42.852833333333336</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>2019</v>
       </c>
@@ -6950,7 +6944,7 @@
         <v>41.47208333333333</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>2019</v>
       </c>
@@ -6976,7 +6970,7 @@
         <v>42.061250000000001</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>2019</v>
       </c>
@@ -7002,7 +6996,7 @@
         <v>42.304791666666667</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>2019</v>
       </c>
@@ -7028,7 +7022,7 @@
         <v>27.315458333333336</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>2020</v>
       </c>
@@ -7054,7 +7048,7 @@
         <v>33.478666666666669</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>2020</v>
       </c>
@@ -7080,7 +7074,7 @@
         <v>27.624333333333336</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>2020</v>
       </c>
@@ -7106,7 +7100,7 @@
         <v>24.963458333333332</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>2020</v>
       </c>
@@ -7132,7 +7126,7 @@
         <v>58.285500000000006</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>2020</v>
       </c>
@@ -7158,7 +7152,7 @@
         <v>53.121833333333335</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>2020</v>
       </c>
@@ -7184,7 +7178,7 @@
         <v>44.085125000000005</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>2020</v>
       </c>
@@ -7210,7 +7204,7 @@
         <v>33.72775</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>2020</v>
       </c>
@@ -7236,7 +7230,7 @@
         <v>26.080833333333334</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>2020</v>
       </c>
@@ -7262,7 +7256,7 @@
         <v>25.158291666666667</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>2020</v>
       </c>
@@ -7288,7 +7282,7 @@
         <v>32.530750000000005</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>2020</v>
       </c>
@@ -7314,7 +7308,7 @@
         <v>31.543166666666668</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>2020</v>
       </c>
@@ -7340,7 +7334,7 @@
         <v>41.186833333333333</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>2021</v>
       </c>
@@ -7366,7 +7360,7 @@
         <v>39.987499999999997</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>2021</v>
       </c>
@@ -7392,7 +7386,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>2021</v>
       </c>
@@ -7418,7 +7412,7 @@
         <v>51.742833333333337</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>2021</v>
       </c>
@@ -7444,7 +7438,7 @@
         <v>32.895333333333333</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>2021</v>
       </c>
@@ -7470,7 +7464,7 @@
         <v>40.373374999999996</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>2021</v>
       </c>
@@ -7496,7 +7490,7 @@
         <v>35.452666666666666</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>2021</v>
       </c>
@@ -7522,7 +7516,7 @@
         <v>24.681999999999999</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>2021</v>
       </c>
@@ -7548,7 +7542,7 @@
         <v>28.134458333333335</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>2021</v>
       </c>
@@ -7574,7 +7568,7 @@
         <v>22.558083333333336</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>2021</v>
       </c>
@@ -7597,7 +7591,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>2021</v>
       </c>
@@ -7620,7 +7614,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>2021</v>
       </c>
@@ -7643,7 +7637,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>2022</v>
       </c>
@@ -7666,7 +7660,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>2022</v>
       </c>
@@ -7689,7 +7683,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>2022</v>
       </c>
@@ -7712,7 +7706,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>2022</v>
       </c>
@@ -7735,7 +7729,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>2022</v>
       </c>
@@ -7758,7 +7752,7 @@
         <v>73.009416666666667</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>2022</v>
       </c>

</xml_diff>